<commit_message>
topics again and vis
</commit_message>
<xml_diff>
--- a/data/topic_model_data/topics_and_sentiment_8-1.xlsx
+++ b/data/topic_model_data/topics_and_sentiment_8-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paigelee/Desktop/summer2022/stanford/research/ukraine-media-CSLI/data/topic_model_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5110123-163E-D444-BA89-51BA3D3B6E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBBD10F-5086-EF45-B43E-2613A34B5315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="28560" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,9 +103,6 @@
     <t>support integrity russian west noted political ukraines sovereignty border added concerned</t>
   </si>
   <si>
-    <t>Ukrainian Sovereignty (E-W)</t>
-  </si>
-  <si>
     <t>sanctions russia swift new banks eu restrictions individuals menendez western target</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>Russian-Western</t>
+  </si>
+  <si>
+    <t>Ukrainian Sovereignty</t>
   </si>
 </sst>
 </file>
@@ -267,12 +267,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -303,7 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -322,12 +328,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -345,16 +352,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -694,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -727,7 +724,7 @@
         <v>12</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>13</v>
@@ -822,10 +819,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
       </c>
       <c r="E3" s="7">
         <v>-7.7506746626686579E-2</v>
@@ -876,10 +873,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
         <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
       </c>
       <c r="E4" s="7">
         <v>-1.13508459483526E-2</v>
@@ -930,10 +927,10 @@
         <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
         <v>54</v>
-      </c>
-      <c r="D5" t="s">
-        <v>55</v>
       </c>
       <c r="E5" s="7">
         <v>-6.0331047992164398E-2</v>
@@ -1038,10 +1035,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
       </c>
       <c r="E7" s="7">
         <v>1.101173512154228E-2</v>
@@ -1092,10 +1089,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
         <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
       </c>
       <c r="E8" s="7">
         <v>-4.9586326767091557E-2</v>
@@ -1146,10 +1143,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
         <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
       </c>
       <c r="E9" s="7">
         <v>2.9384615384615148E-3</v>
@@ -1200,10 +1197,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
         <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
       </c>
       <c r="E10" s="7">
         <v>-5.2392273402674661E-3</v>
@@ -1254,10 +1251,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
         <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
       </c>
       <c r="E11" s="7">
         <v>2.1372964169381139E-2</v>
@@ -1310,7 +1307,7 @@
       <c r="C12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="7">
@@ -1362,10 +1359,10 @@
         <v>24</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" t="s">
         <v>64</v>
-      </c>
-      <c r="D13" t="s">
-        <v>65</v>
       </c>
       <c r="E13" s="7">
         <v>3.4850318471337571E-2</v>
@@ -1470,10 +1467,10 @@
         <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
         <v>46</v>
-      </c>
-      <c r="D15" t="s">
-        <v>47</v>
       </c>
       <c r="E15" s="7">
         <v>-5.3762195121951198E-2</v>
@@ -1524,10 +1521,10 @@
         <v>11</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>39</v>
       </c>
       <c r="E16" s="7">
         <v>-3.5071651090342618E-2</v>
@@ -1578,10 +1575,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
         <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
       </c>
       <c r="E17" s="7">
         <v>4.7818181818181787E-3</v>
@@ -1632,10 +1629,10 @@
         <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
         <v>56</v>
-      </c>
-      <c r="D18" t="s">
-        <v>57</v>
       </c>
       <c r="E18" s="7">
         <v>-2.9129471890971041E-2</v>
@@ -1686,10 +1683,10 @@
         <v>9</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
         <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>35</v>
       </c>
       <c r="E19" s="7">
         <v>2.0102189781021899E-2</v>
@@ -1740,10 +1737,10 @@
         <v>21</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="D20" t="s">
-        <v>59</v>
       </c>
       <c r="E20" s="7">
         <v>2.7573221757322169E-2</v>
@@ -1794,10 +1791,10 @@
         <v>14</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
         <v>44</v>
-      </c>
-      <c r="D21" t="s">
-        <v>45</v>
       </c>
       <c r="E21" s="7">
         <v>-2.878947368421059E-2</v>
@@ -1850,8 +1847,8 @@
       <c r="C22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D22" t="s">
-        <v>23</v>
+      <c r="D22" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="E22" s="7">
         <v>1.6763546798029539E-2</v>
@@ -1902,10 +1899,10 @@
         <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" t="s">
         <v>52</v>
-      </c>
-      <c r="D23" t="s">
-        <v>53</v>
       </c>
       <c r="E23" s="7">
         <v>-3.3360000000000008E-2</v>
@@ -1956,10 +1953,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
         <v>48</v>
-      </c>
-      <c r="D24" t="s">
-        <v>49</v>
       </c>
       <c r="E24" s="7">
         <v>-8.2091623036649242E-2</v>
@@ -2010,10 +2007,10 @@
         <v>22</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="D25" t="s">
-        <v>61</v>
       </c>
       <c r="E25" s="7">
         <v>-0.1523076923076925</v>
@@ -2064,10 +2061,10 @@
         <v>23</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="D26" t="s">
-        <v>63</v>
       </c>
       <c r="E26" s="7">
         <v>-4.9753246753246792E-2</v>
@@ -2118,10 +2115,10 @@
         <v>17</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" t="s">
         <v>50</v>
-      </c>
-      <c r="D27" t="s">
-        <v>51</v>
       </c>
       <c r="E27" s="7">
         <v>-1.406249999999776E-4</v>
@@ -2165,8 +2162,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q28">
-    <sortCondition descending="1" ref="M1:M28"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q30">
+    <sortCondition descending="1" ref="M1:M30"/>
   </sortState>
   <conditionalFormatting sqref="E2:I27">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
@@ -2177,5 +2174,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>